<commit_message>
Add sequential experiments, live figures
</commit_message>
<xml_diff>
--- a/Experiment.xlsx
+++ b/Experiment.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a688d21030416907/Documents/GitHub/auto-LNP/auto-LNP/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6B5611A3-19D5-4827-BD2B-085EFE5A0B72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="16" documentId="8_{6B5611A3-19D5-4827-BD2B-085EFE5A0B72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{588CD6F2-EE8F-44D7-B9EA-81FC27308DBA}"/>
   <bookViews>
-    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{9BC798F6-E318-4A3F-8CD0-9B89A2D71B32}"/>
+    <workbookView xWindow="15135" yWindow="0" windowWidth="13770" windowHeight="15585" xr2:uid="{9BC798F6-E318-4A3F-8CD0-9B89A2D71B32}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>Number</t>
   </si>
@@ -51,9 +51,6 @@
   </si>
   <si>
     <t>FR4</t>
-  </si>
-  <si>
-    <t>Volume</t>
   </si>
 </sst>
 </file>
@@ -405,15 +402,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BBA571AF-EB09-4360-B555-AB34E4DA0463}">
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -429,8 +426,38 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
-        <v>5</v>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>50</v>
+      </c>
+      <c r="C2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>10</v>
+      </c>
+      <c r="C3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="C4">
+        <v>10</v>
+      </c>
+      <c r="D4">
+        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>